<commit_message>
docs deel 2 (checklist, poster, dossier)
</commit_message>
<xml_diff>
--- a/docs/timesheet_Dylan_VanSteirteghem.xlsx
+++ b/docs/timesheet_Dylan_VanSteirteghem.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dylan/qawaq_repository/qawaq.local/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dylan/Git/nmdad2ek2qawaq/nmdad2.local/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>angular store vullen met faker, zoeken naar manier om winkelmandje te vullen</t>
+  </si>
+  <si>
+    <t>&lt;- EK2 restart</t>
+  </si>
+  <si>
+    <t>opnieuw beginnen: databases, views, controllers</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>42618</v>
       </c>
@@ -689,63 +695,75 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>42592</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="7">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>42593</v>
+      </c>
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="C32" s="7"/>
     </row>
@@ -758,7 +776,7 @@
       </c>
       <c r="C33" s="8">
         <f>SUM(C3:C32)</f>
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
docs deel 3 (poster tweede try)
</commit_message>
<xml_diff>
--- a/docs/timesheet_Dylan_VanSteirteghem.xlsx
+++ b/docs/timesheet_Dylan_VanSteirteghem.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Datum</t>
   </si>
@@ -95,7 +95,25 @@
     <t>&lt;- EK2 restart</t>
   </si>
   <si>
-    <t>opnieuw beginnen: databases, views, controllers</t>
+    <t>functies CRUD in backoffice voor producten, eerste werken aan app</t>
+  </si>
+  <si>
+    <t>Api en routes api voor communicatie met app, customers backoffice</t>
+  </si>
+  <si>
+    <t>orders toevoegen via app, opschonen app</t>
+  </si>
+  <si>
+    <t>inloggen op app, producten weergeven en api, database voor orders, CRUD voor customer op app</t>
+  </si>
+  <si>
+    <t>opnieuw beginnen: databases, views, controllers, factories met faker, databases geseed.</t>
+  </si>
+  <si>
+    <t>proberen statistieken weergeven op dashboard, order overzicht klant, github repo herstarten, docs bijwerken</t>
+  </si>
+  <si>
+    <t>Presentatie, Dossier aanvullen, poster, checklist, finale versie klaarzetten</t>
   </si>
 </sst>
 </file>
@@ -498,13 +516,13 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="2" max="2" width="88" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -700,7 +718,7 @@
         <v>42592</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C18" s="7">
         <v>8</v>
@@ -713,27 +731,67 @@
       <c r="A19" s="5">
         <v>42593</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="5">
+        <v>42594</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="5">
+        <v>42595</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="7">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="5">
+        <v>42596</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="7">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="5">
+        <v>42597</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="7">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="5">
+        <v>42598</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="7">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
@@ -776,7 +834,7 @@
       </c>
       <c r="C33" s="8">
         <f>SUM(C3:C32)</f>
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>

</xml_diff>